<commit_message>
update routes with new info, also remove old chart
</commit_message>
<xml_diff>
--- a/komorantags/Korean POS tags comparison chart.xlsx
+++ b/komorantags/Korean POS tags comparison chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inhwamo/Documents/grammarlycjk/komorantags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FC0559-4D54-6C4E-8767-02C839395D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975CEB94-EC2C-3D47-BD45-8A26D6B564D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1655,7 +1655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1741,6 +1741,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2082,9 +2085,9 @@
   </sheetPr>
   <dimension ref="A1:AK1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y16" sqref="Y16:Y17"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3881,7 +3884,7 @@
       <c r="X35" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="Y35" s="18" t="s">
+      <c r="Y35" s="43" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4034,7 +4037,7 @@
       <c r="X38" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="Y38" s="18" t="s">
+      <c r="Y38" s="43" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4332,7 +4335,7 @@
       <c r="V44" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="W44" s="2" t="s">
+      <c r="W44" s="41" t="s">
         <v>215</v>
       </c>
       <c r="X44" s="32" t="s">

</xml_diff>